<commit_message>
All Emissions from Emissionskatalog.xlsx in DB
</commit_message>
<xml_diff>
--- a/app/static/data/Emissionskatalog.xlsx
+++ b/app/static/data/Emissionskatalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16620" windowHeight="5010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16620" windowHeight="5016"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="126">
   <si>
     <t>category</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>emissions</t>
+  </si>
+  <si>
+    <t>https://www.zwei-grad-eine-tonne.at/hintergrund-berechnungen/abschnitt-i-lustvoll-die-welt-retten</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="9">
           <cell r="B9">
@@ -1022,23 +1025,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80:E200"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -1077,9 +1080,12 @@
       <c r="F2" s="4">
         <v>420</v>
       </c>
+      <c r="G2" t="s">
+        <v>125</v>
+      </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -1092,9 +1098,12 @@
       <c r="F3" s="4">
         <v>1680</v>
       </c>
+      <c r="G3" t="s">
+        <v>125</v>
+      </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -1107,9 +1116,12 @@
       <c r="F4" s="4">
         <v>0</v>
       </c>
+      <c r="G4" t="s">
+        <v>125</v>
+      </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -1122,9 +1134,12 @@
       <c r="F5" s="4">
         <v>70</v>
       </c>
+      <c r="G5" t="s">
+        <v>125</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -1137,9 +1152,12 @@
       <c r="F6" s="4">
         <v>4</v>
       </c>
+      <c r="G6" t="s">
+        <v>125</v>
+      </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -1152,9 +1170,12 @@
       <c r="F7" s="4">
         <v>378</v>
       </c>
+      <c r="G7" t="s">
+        <v>125</v>
+      </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>110</v>
       </c>
@@ -1167,9 +1188,12 @@
       <c r="F8" s="4">
         <v>420</v>
       </c>
+      <c r="G8" t="s">
+        <v>125</v>
+      </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -1182,9 +1206,12 @@
       <c r="F9" s="4">
         <v>189</v>
       </c>
+      <c r="G9" t="s">
+        <v>125</v>
+      </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -1197,9 +1224,12 @@
       <c r="F10" s="4">
         <v>581.53846153846143</v>
       </c>
+      <c r="G10" t="s">
+        <v>125</v>
+      </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -1212,9 +1242,12 @@
       <c r="F11" s="4">
         <v>700</v>
       </c>
+      <c r="G11" t="s">
+        <v>125</v>
+      </c>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -1227,9 +1260,12 @@
       <c r="F12" s="4">
         <v>210</v>
       </c>
+      <c r="G12" t="s">
+        <v>125</v>
+      </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -1242,9 +1278,12 @@
       <c r="F13" s="4">
         <v>70</v>
       </c>
+      <c r="G13" t="s">
+        <v>125</v>
+      </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>110</v>
       </c>
@@ -1257,9 +1296,12 @@
       <c r="F14" s="4">
         <v>35</v>
       </c>
+      <c r="G14" t="s">
+        <v>125</v>
+      </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>110</v>
       </c>
@@ -1272,9 +1314,12 @@
       <c r="F15" s="4">
         <v>112</v>
       </c>
+      <c r="G15" t="s">
+        <v>125</v>
+      </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -1287,9 +1332,12 @@
       <c r="F16" s="4">
         <v>168</v>
       </c>
+      <c r="G16" t="s">
+        <v>125</v>
+      </c>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -1302,9 +1350,12 @@
       <c r="F17" s="4">
         <v>56</v>
       </c>
+      <c r="G17" t="s">
+        <v>125</v>
+      </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>110</v>
       </c>
@@ -1317,9 +1368,12 @@
       <c r="F18" s="4">
         <v>26.25</v>
       </c>
+      <c r="G18" t="s">
+        <v>125</v>
+      </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -1332,9 +1386,12 @@
       <c r="F19" s="4">
         <v>63</v>
       </c>
+      <c r="G19" t="s">
+        <v>125</v>
+      </c>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>110</v>
       </c>
@@ -1347,9 +1404,12 @@
       <c r="F20" s="4">
         <v>10.5</v>
       </c>
+      <c r="G20" t="s">
+        <v>125</v>
+      </c>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>110</v>
       </c>
@@ -1362,9 +1422,12 @@
       <c r="F21" s="4">
         <v>63</v>
       </c>
+      <c r="G21" t="s">
+        <v>125</v>
+      </c>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>110</v>
       </c>
@@ -1377,9 +1440,12 @@
       <c r="F22" s="4">
         <v>1517.7884615384617</v>
       </c>
+      <c r="G22" t="s">
+        <v>125</v>
+      </c>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -1392,9 +1458,12 @@
       <c r="F23" s="4">
         <v>207.00000000000003</v>
       </c>
+      <c r="G23" t="s">
+        <v>125</v>
+      </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -1407,9 +1476,12 @@
       <c r="F24" s="4">
         <v>3031</v>
       </c>
+      <c r="G24" t="s">
+        <v>125</v>
+      </c>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>110</v>
       </c>
@@ -1422,9 +1494,12 @@
       <c r="F25" s="4">
         <v>500.50000000000006</v>
       </c>
+      <c r="G25" t="s">
+        <v>125</v>
+      </c>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1440,8 +1515,11 @@
       <c r="F26" s="3">
         <v>5121.4851071999992</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1457,8 +1535,11 @@
       <c r="F27" s="3">
         <v>2358.3698208000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1474,8 +1555,11 @@
       <c r="F28" s="3">
         <v>1042.7266080000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1491,8 +1575,11 @@
       <c r="F29" s="3">
         <v>104.27266080000004</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1508,8 +1595,11 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1525,8 +1615,11 @@
       <c r="F31">
         <v>620</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1542,8 +1635,11 @@
       <c r="F32" s="4">
         <v>2556.3054558212552</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1559,8 +1655,11 @@
       <c r="F33">
         <v>1022.0000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>30</v>
       </c>
@@ -1576,8 +1675,11 @@
       <c r="F34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1593,8 +1695,11 @@
       <c r="F35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1610,8 +1715,11 @@
       <c r="F36">
         <v>432</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1628,8 +1736,11 @@
         <f>'[1]Fitness-Center'!$B$22</f>
         <v>141.86559429590017</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1646,8 +1757,11 @@
         <f>[1]Schifahren!$B$9</f>
         <v>157.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1663,8 +1777,11 @@
       <c r="F39">
         <v>200</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1681,8 +1798,11 @@
         <f>[1]Schwimmen!$B$9</f>
         <v>180</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -1699,8 +1819,11 @@
         <f>[1]Motorradfahren!$B$8</f>
         <v>420.37500000000006</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -1717,8 +1840,11 @@
         <f>[1]Gastronomie!$B$19</f>
         <v>170</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -1735,8 +1861,11 @@
         <f>[1]Internetnutzung!$B$11</f>
         <v>58.18181818181818</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1752,8 +1881,11 @@
       <c r="F44" s="4">
         <v>2000</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -1766,8 +1898,11 @@
       <c r="F45" s="4">
         <v>1300</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -1785,8 +1920,11 @@
         <f>[2]Urlaubsverhalten!$H$6</f>
         <v>280</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -1804,8 +1942,11 @@
         <f>[2]Urlaubsverhalten!$H$10</f>
         <v>645</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -1823,8 +1964,11 @@
         <f>[2]Urlaubsverhalten!$H$14</f>
         <v>2030</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -1842,8 +1986,11 @@
         <f>[2]Urlaubsverhalten!$H$17</f>
         <v>210</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -1861,8 +2008,11 @@
         <f>[2]Urlaubsverhalten!$H$21</f>
         <v>105</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -1878,8 +2028,11 @@
       <c r="F51">
         <v>280</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -1895,8 +2048,11 @@
       <c r="F52">
         <v>420</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -1912,8 +2068,11 @@
       <c r="F53">
         <v>225</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -1929,8 +2088,11 @@
       <c r="F54">
         <v>1120</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -1946,8 +2108,11 @@
       <c r="F55">
         <v>910</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -1963,8 +2128,11 @@
       <c r="F56">
         <v>210</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -1980,8 +2148,11 @@
       <c r="F57">
         <v>52.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -1997,8 +2168,11 @@
       <c r="F58">
         <v>52.5</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -2014,8 +2188,11 @@
       <c r="F59">
         <v>450.2</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -2031,8 +2208,11 @@
       <c r="F60">
         <v>488.8</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -2048,8 +2228,11 @@
       <c r="F61">
         <v>40.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -2065,8 +2248,11 @@
       <c r="F62">
         <v>74.8</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2082,8 +2268,11 @@
       <c r="F63">
         <v>119.8</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2099,8 +2288,11 @@
       <c r="F64">
         <v>171.6</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -2116,8 +2308,11 @@
       <c r="F65">
         <v>407.9</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -2133,8 +2328,11 @@
       <c r="F66">
         <v>1753.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -2151,8 +2349,11 @@
         <f>F66-700</f>
         <v>1053.5999999999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>63</v>
       </c>
@@ -2169,8 +2370,11 @@
         <f>F66-300</f>
         <v>1453.6</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>63</v>
       </c>
@@ -2186,8 +2390,11 @@
       <c r="F69">
         <v>800</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -2203,8 +2410,11 @@
       <c r="F70">
         <v>400</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>93</v>
       </c>
@@ -2221,8 +2431,11 @@
         <f>'[3]Sonstiger Konsum'!$B$7</f>
         <v>385</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>93</v>
       </c>
@@ -2239,8 +2452,11 @@
         <f>'[3]Sonstiger Konsum'!$B$11</f>
         <v>420</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>93</v>
       </c>
@@ -2257,8 +2473,11 @@
         <f>'[3]Sonstiger Konsum'!$B$15</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>93</v>
       </c>
@@ -2275,8 +2494,11 @@
         <f>'[3]Sonstiger Konsum'!$B$21</f>
         <v>218</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>93</v>
       </c>
@@ -2293,8 +2515,11 @@
         <f>'[3]Sonstiger Konsum'!$B$25</f>
         <v>192.5</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>93</v>
       </c>
@@ -2311,8 +2536,11 @@
         <f>'[3]Sonstiger Konsum'!$B$27</f>
         <v>1515.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>104</v>
       </c>
@@ -2328,8 +2556,11 @@
       <c r="F77">
         <v>600</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>105</v>
       </c>
@@ -2345,8 +2576,11 @@
       <c r="F78">
         <v>1900</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
         <v>108</v>
       </c>
@@ -2362,8 +2596,11 @@
       <c r="F79">
         <v>1900</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>63</v>
       </c>
@@ -2379,8 +2616,11 @@
       <c r="F80">
         <v>1800</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>110</v>
       </c>
@@ -2396,8 +2636,11 @@
       <c r="F81">
         <v>1500</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>111</v>
       </c>
@@ -2413,8 +2656,11 @@
       <c r="F82">
         <v>600</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -2430,8 +2676,11 @@
       <c r="F83">
         <v>600</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -2447,8 +2696,11 @@
       <c r="F84">
         <v>300</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>36</v>
       </c>
@@ -2464,8 +2716,11 @@
       <c r="F85">
         <v>900</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>30</v>
       </c>
@@ -2481,8 +2736,11 @@
       <c r="F86">
         <v>400</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -2498,8 +2756,11 @@
       <c r="F87">
         <v>1500</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>104</v>
       </c>
@@ -2515,8 +2776,11 @@
       <c r="F88">
         <v>600</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>105</v>
       </c>
@@ -2532,8 +2796,11 @@
       <c r="F89">
         <v>1900</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>108</v>
       </c>
@@ -2549,8 +2816,11 @@
       <c r="F90">
         <v>1900</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>63</v>
       </c>
@@ -2566,8 +2836,11 @@
       <c r="F91">
         <v>1700</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>110</v>
       </c>
@@ -2583,8 +2856,11 @@
       <c r="F92">
         <v>1500</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>111</v>
       </c>
@@ -2600,8 +2876,11 @@
       <c r="F93">
         <v>500</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -2617,8 +2896,11 @@
       <c r="F94">
         <v>500</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -2634,8 +2916,11 @@
       <c r="F95">
         <v>300</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>36</v>
       </c>
@@ -2651,8 +2936,11 @@
       <c r="F96">
         <v>700</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>30</v>
       </c>
@@ -2668,8 +2956,11 @@
       <c r="F97">
         <v>900</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>93</v>
       </c>
@@ -2685,8 +2976,11 @@
       <c r="F98">
         <v>1400</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>104</v>
       </c>
@@ -2702,8 +2996,11 @@
       <c r="F99">
         <v>600</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>105</v>
       </c>
@@ -2719,8 +3016,11 @@
       <c r="F100">
         <v>2000</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G100" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>108</v>
       </c>
@@ -2736,8 +3036,11 @@
       <c r="F101">
         <v>1900</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G101" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>63</v>
       </c>
@@ -2753,8 +3056,11 @@
       <c r="F102">
         <v>700</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>110</v>
       </c>
@@ -2770,8 +3076,11 @@
       <c r="F103">
         <v>500</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G103" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -2787,8 +3096,11 @@
       <c r="F104">
         <v>200</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>3</v>
       </c>
@@ -2804,8 +3116,11 @@
       <c r="F105">
         <v>100</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -2821,8 +3136,11 @@
       <c r="F106">
         <v>200</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G106" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>36</v>
       </c>
@@ -2838,8 +3156,11 @@
       <c r="F107">
         <v>400</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>30</v>
       </c>
@@ -2855,8 +3176,11 @@
       <c r="F108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G108" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>93</v>
       </c>
@@ -2872,8 +3196,11 @@
       <c r="F109">
         <v>1000</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>104</v>
       </c>
@@ -2889,8 +3216,11 @@
       <c r="F110">
         <v>300</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G110" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>105</v>
       </c>
@@ -2906,8 +3236,11 @@
       <c r="F111">
         <v>1800</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G111" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>108</v>
       </c>
@@ -2923,8 +3256,11 @@
       <c r="F112">
         <v>1900</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>63</v>
       </c>
@@ -2940,8 +3276,11 @@
       <c r="F113">
         <v>900</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>110</v>
       </c>
@@ -2957,8 +3296,11 @@
       <c r="F114">
         <v>900</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G114" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>111</v>
       </c>
@@ -2974,8 +3316,11 @@
       <c r="F115">
         <v>400</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G115" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>3</v>
       </c>
@@ -2991,8 +3336,11 @@
       <c r="F116">
         <v>600</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G116" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>16</v>
       </c>
@@ -3008,8 +3356,11 @@
       <c r="F117">
         <v>400</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G117" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>36</v>
       </c>
@@ -3025,8 +3376,11 @@
       <c r="F118">
         <v>600</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G118" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>30</v>
       </c>
@@ -3042,8 +3396,11 @@
       <c r="F119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G119" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>93</v>
       </c>
@@ -3059,8 +3416,11 @@
       <c r="F120">
         <v>1200</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G120" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>104</v>
       </c>
@@ -3076,8 +3436,11 @@
       <c r="F121">
         <v>400</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G121" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>105</v>
       </c>
@@ -3093,8 +3456,11 @@
       <c r="F122">
         <v>2000</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G122" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>108</v>
       </c>
@@ -3110,8 +3476,11 @@
       <c r="F123">
         <v>1900</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G123" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>63</v>
       </c>
@@ -3127,8 +3496,11 @@
       <c r="F124">
         <v>700</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G124" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>110</v>
       </c>
@@ -3144,8 +3516,11 @@
       <c r="F125">
         <v>500</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G125" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>111</v>
       </c>
@@ -3161,8 +3536,11 @@
       <c r="F126">
         <v>200</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G126" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>3</v>
       </c>
@@ -3178,8 +3556,11 @@
       <c r="F127">
         <v>200</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G127" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>16</v>
       </c>
@@ -3195,8 +3576,11 @@
       <c r="F128">
         <v>200</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G128" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>36</v>
       </c>
@@ -3212,8 +3596,11 @@
       <c r="F129">
         <v>600</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G129" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>30</v>
       </c>
@@ -3229,8 +3616,11 @@
       <c r="F130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G130" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>93</v>
       </c>
@@ -3246,8 +3636,11 @@
       <c r="F131">
         <v>700</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G131" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>104</v>
       </c>
@@ -3263,8 +3656,11 @@
       <c r="F132">
         <v>400</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G132" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>105</v>
       </c>
@@ -3280,8 +3676,11 @@
       <c r="F133">
         <v>1900</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G133" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>108</v>
       </c>
@@ -3297,8 +3696,11 @@
       <c r="F134">
         <v>1900</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G134" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>63</v>
       </c>
@@ -3314,8 +3716,11 @@
       <c r="F135">
         <v>900</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G135" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>110</v>
       </c>
@@ -3331,8 +3736,11 @@
       <c r="F136">
         <v>400</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G136" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>111</v>
       </c>
@@ -3348,8 +3756,11 @@
       <c r="F137">
         <v>200</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G137" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>3</v>
       </c>
@@ -3365,8 +3776,11 @@
       <c r="F138">
         <v>100</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G138" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>16</v>
       </c>
@@ -3382,8 +3796,11 @@
       <c r="F139">
         <v>100</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G139" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>36</v>
       </c>
@@ -3399,8 +3816,11 @@
       <c r="F140">
         <v>700</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G140" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>30</v>
       </c>
@@ -3416,8 +3836,11 @@
       <c r="F141">
         <v>300</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G141" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>93</v>
       </c>
@@ -3433,8 +3856,11 @@
       <c r="F142">
         <v>900</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G142" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>104</v>
       </c>
@@ -3450,8 +3876,11 @@
       <c r="F143">
         <v>300</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G143" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>105</v>
       </c>
@@ -3467,8 +3896,11 @@
       <c r="F144">
         <v>1900</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G144" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>108</v>
       </c>
@@ -3484,8 +3916,11 @@
       <c r="F145">
         <v>1900</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G145" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>63</v>
       </c>
@@ -3501,8 +3936,11 @@
       <c r="F146">
         <v>1200</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G146" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>110</v>
       </c>
@@ -3518,8 +3956,11 @@
       <c r="F147">
         <v>1000</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G147" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>111</v>
       </c>
@@ -3535,8 +3976,11 @@
       <c r="F148">
         <v>400</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G148" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>3</v>
       </c>
@@ -3552,8 +3996,11 @@
       <c r="F149">
         <v>300</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G149" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>16</v>
       </c>
@@ -3569,8 +4016,11 @@
       <c r="F150">
         <v>200</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G150" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>36</v>
       </c>
@@ -3586,8 +4036,11 @@
       <c r="F151">
         <v>600</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G151" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>30</v>
       </c>
@@ -3603,8 +4056,11 @@
       <c r="F152">
         <v>400</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G152" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>93</v>
       </c>
@@ -3620,8 +4076,11 @@
       <c r="F153">
         <v>1100</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G153" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>104</v>
       </c>
@@ -3637,8 +4096,11 @@
       <c r="F154">
         <v>300</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G154" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>105</v>
       </c>
@@ -3654,8 +4116,11 @@
       <c r="F155">
         <v>1800</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G155" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>108</v>
       </c>
@@ -3671,8 +4136,11 @@
       <c r="F156">
         <v>1900</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G156" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>63</v>
       </c>
@@ -3688,8 +4156,11 @@
       <c r="F157">
         <v>300</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G157" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>110</v>
       </c>
@@ -3705,8 +4176,11 @@
       <c r="F158">
         <v>200</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G158" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>111</v>
       </c>
@@ -3722,8 +4196,11 @@
       <c r="F159">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G159" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>3</v>
       </c>
@@ -3739,8 +4216,11 @@
       <c r="F160">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G160" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>16</v>
       </c>
@@ -3756,8 +4236,11 @@
       <c r="F161">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G161" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>36</v>
       </c>
@@ -3773,8 +4256,11 @@
       <c r="F162">
         <v>400</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G162" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>30</v>
       </c>
@@ -3790,8 +4276,11 @@
       <c r="F163">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G163" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>93</v>
       </c>
@@ -3807,8 +4296,11 @@
       <c r="F164">
         <v>700</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G164" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>104</v>
       </c>
@@ -3824,8 +4316,11 @@
       <c r="F165">
         <v>300</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G165" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>105</v>
       </c>
@@ -3841,8 +4336,11 @@
       <c r="F166">
         <v>1600</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G166" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>108</v>
       </c>
@@ -3858,8 +4356,11 @@
       <c r="F167">
         <v>1900</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G167" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>63</v>
       </c>
@@ -3875,8 +4376,11 @@
       <c r="F168">
         <v>900</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G168" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>110</v>
       </c>
@@ -3892,8 +4396,11 @@
       <c r="F169">
         <v>500</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G169" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>111</v>
       </c>
@@ -3909,8 +4416,11 @@
       <c r="F170">
         <v>200</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G170" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>3</v>
       </c>
@@ -3926,8 +4436,11 @@
       <c r="F171">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G171" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>16</v>
       </c>
@@ -3943,8 +4456,11 @@
       <c r="F172">
         <v>100</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G172" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>36</v>
       </c>
@@ -3960,8 +4476,11 @@
       <c r="F173">
         <v>500</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G173" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>30</v>
       </c>
@@ -3977,8 +4496,11 @@
       <c r="F174">
         <v>300</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G174" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>93</v>
       </c>
@@ -3994,8 +4516,11 @@
       <c r="F175">
         <v>800</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G175" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>104</v>
       </c>
@@ -4011,8 +4536,11 @@
       <c r="F176">
         <v>400</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G176" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>105</v>
       </c>
@@ -4028,8 +4556,11 @@
       <c r="F177">
         <v>1700</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G177" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>108</v>
       </c>
@@ -4045,8 +4576,11 @@
       <c r="F178">
         <v>1900</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G178" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>63</v>
       </c>
@@ -4062,8 +4596,11 @@
       <c r="F179">
         <v>1200</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G179" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>110</v>
       </c>
@@ -4079,8 +4616,11 @@
       <c r="F180">
         <v>900</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G180" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>111</v>
       </c>
@@ -4096,8 +4636,11 @@
       <c r="F181">
         <v>500</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G181" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>3</v>
       </c>
@@ -4113,8 +4656,11 @@
       <c r="F182">
         <v>600</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G182" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>16</v>
       </c>
@@ -4130,8 +4676,11 @@
       <c r="F183">
         <v>200</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G183" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>36</v>
       </c>
@@ -4147,8 +4696,11 @@
       <c r="F184">
         <v>900</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G184" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>30</v>
       </c>
@@ -4164,8 +4716,11 @@
       <c r="F185">
         <v>400</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G185" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>93</v>
       </c>
@@ -4181,8 +4736,11 @@
       <c r="F186">
         <v>1300</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G186" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>104</v>
       </c>
@@ -4198,8 +4756,11 @@
       <c r="F187">
         <v>500</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G187" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>105</v>
       </c>
@@ -4215,8 +4776,11 @@
       <c r="F188">
         <v>1800</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G188" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>108</v>
       </c>
@@ -4232,8 +4796,11 @@
       <c r="F189">
         <v>1900</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G189" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>63</v>
       </c>
@@ -4249,8 +4816,11 @@
       <c r="F190">
         <v>1200</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G190" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>110</v>
       </c>
@@ -4266,8 +4836,11 @@
       <c r="F191">
         <v>900</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G191" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>111</v>
       </c>
@@ -4283,8 +4856,11 @@
       <c r="F192">
         <v>300</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G192" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>3</v>
       </c>
@@ -4300,8 +4876,11 @@
       <c r="F193">
         <v>500</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G193" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>16</v>
       </c>
@@ -4317,8 +4896,11 @@
       <c r="F194">
         <v>300</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G194" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>36</v>
       </c>
@@ -4334,8 +4916,11 @@
       <c r="F195">
         <v>600</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G195" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>30</v>
       </c>
@@ -4351,8 +4936,11 @@
       <c r="F196">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G196" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>93</v>
       </c>
@@ -4368,8 +4956,11 @@
       <c r="F197">
         <v>900</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G197" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>104</v>
       </c>
@@ -4385,8 +4976,11 @@
       <c r="F198">
         <v>500</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G198" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>105</v>
       </c>
@@ -4402,8 +4996,11 @@
       <c r="F199">
         <v>1600</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G199" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>108</v>
       </c>
@@ -4418,6 +5015,9 @@
       </c>
       <c r="F200">
         <v>1900</v>
+      </c>
+      <c r="G200" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>